<commit_message>
Fecha en el acta de recepcion y respaldo
</commit_message>
<xml_diff>
--- a/php/report/plantilla_acta_recepcion.xlsx
+++ b/php/report/plantilla_acta_recepcion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\InventarioISTGTest\php\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1332DE13-C7C0-4E47-B109-F5E69BF1E118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444F4EED-719B-4B26-8242-073E4BE19B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Segunda.- En caso de cambio o retiro, el custodio de los bienes deberá legalizar la respectiva acta de descarga a nombre de la persona quien se responsabilizará, para su actualización registro y control.</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t xml:space="preserve">Primera.- Los bienes descritos en la presente acta, a partir de la firma, estarán bajo la responsabilidad, buen uso y cuidado de quien recibe  y garantiza que se emplearán única y exclusivamente para cumplir con los fines propios inherentes  a las funciones que se cumple en en el ISTG </t>
-  </si>
-  <si>
-    <t>En la ciudad de Guayaquil, Provincia de Guayas a los ______ días del mes de _____ de _____, en las oficinas del ISTG, ubicadas _______________________________ se reúnen por una parte_______________________, en calidad de Custodio Administrativo, y quien recibe ________________, quien labora físicamente en  el ISTG  con cargo de ________________con el fin de realizar el acta de entrega recepción de los bienes que se detalla a continuación, conforme lo indica el reglamento general para la Administración, Utilización, Manejo y Control de los bienes e inventarios del sector público en su capítulo III, Art. 41.</t>
   </si>
   <si>
     <t>CODIGO  ITEN ISTG</t>
@@ -678,7 +675,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -821,15 +818,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1273,7 +1261,7 @@
   <dimension ref="A3:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A11" sqref="A11:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,18 +1344,16 @@
       <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="57"/>
+      <c r="A11" s="58"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="60"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
     </row>
@@ -1383,22 +1369,22 @@
       <c r="A14" s="45"/>
       <c r="B14" s="45"/>
       <c r="C14" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="E14" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="F14" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="G14" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="H14" s="31" t="s">
         <v>25</v>
-      </c>
-      <c r="H14" s="31" t="s">
-        <v>26</v>
       </c>
       <c r="I14" s="31" t="s">
         <v>10</v>
@@ -1410,7 +1396,7 @@
       <c r="A15" s="46"/>
       <c r="B15" s="46"/>
       <c r="C15" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
@@ -1466,61 +1452,61 @@
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="59"/>
-      <c r="J20" s="60"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="57"/>
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="61" t="s">
+      <c r="A21" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="62"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="63"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="60"/>
     </row>
     <row r="22" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="62"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="63"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="60"/>
     </row>
     <row r="23" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="61" t="s">
+      <c r="A23" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="62"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="63"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="60"/>
     </row>
     <row r="24" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="42"/>
@@ -1535,32 +1521,32 @@
       <c r="J24" s="44"/>
     </row>
     <row r="25" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="61" t="s">
+      <c r="A25" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="62"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="62"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="63"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="60"/>
     </row>
     <row r="26" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="61" t="s">
+      <c r="A26" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="62"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="63"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="60"/>
     </row>
     <row r="27" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
@@ -1636,17 +1622,17 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
-      <c r="B34" s="66"/>
-      <c r="C34" s="65"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="62"/>
       <c r="D34" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="65"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="65" t="s">
+      <c r="E34" s="62"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="H34" s="65"/>
+      <c r="H34" s="62"/>
       <c r="I34" s="1"/>
       <c r="J34" s="22"/>
     </row>
@@ -1677,8 +1663,8 @@
       <c r="D36" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="E36" s="65"/>
-      <c r="F36" s="65"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="62"/>
       <c r="G36" s="53" t="s">
         <v>15</v>
       </c>
@@ -1694,10 +1680,10 @@
         <v>16</v>
       </c>
       <c r="E37" s="1"/>
-      <c r="G37" s="64" t="s">
+      <c r="G37" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="H37" s="64"/>
+      <c r="H37" s="61"/>
       <c r="J37" s="15"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>